<commit_message>
mulitple excel sheet task done
</commit_message>
<xml_diff>
--- a/TestData/Stage_data.xlsx
+++ b/TestData/Stage_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>testCaseID</t>
   </si>
@@ -35,7 +35,7 @@
     <t>project_Label_updated</t>
   </si>
   <si>
-    <t>testCaseID_01</t>
+    <t>Project_testCaseID_01</t>
   </si>
   <si>
     <t>P40</t>
@@ -47,9 +47,6 @@
     <t>P30</t>
   </si>
   <si>
-    <t>testCaseID2</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -86,7 +83,7 @@
     <t>Skew</t>
   </si>
   <si>
-    <t>testCaseID_02</t>
+    <t>Bridge_testCaseID_02</t>
   </si>
   <si>
     <t>Parabola</t>
@@ -100,13 +97,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +121,12 @@
     <font>
       <sz val="10"/>
       <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -147,39 +150,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,6 +197,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -241,6 +229,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -256,6 +252,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -264,14 +274,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -292,37 +295,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,145 +469,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,35 +486,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -583,153 +557,182 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -746,13 +749,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1080,12 +1083,12 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="13.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="20.5714285714286" customWidth="1"/>
     <col min="2" max="2" width="11.8571428571429" customWidth="1"/>
     <col min="3" max="3" width="15.8571428571429" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
@@ -1144,7 +1147,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1161,48 +1164,48 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="5">
         <v>45237</v>
@@ -1214,19 +1217,19 @@
         <v>14000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2">
         <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J2" s="2">
         <v>1400</v>
@@ -1238,7 +1241,7 @@
         <v>1500</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>